<commit_message>
case study chapter 2 updated
</commit_message>
<xml_diff>
--- a/Class Demo Files/Excel Ch2b/BansalDikshaTravel.xlsx
+++ b/Class Demo Files/Excel Ch2b/BansalDikshaTravel.xlsx
@@ -11,7 +11,7 @@
   </sheets>
   <definedNames>
     <definedName name="Deals">'New Clients'!$A$20:$C$24</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'New Clients'!$D$13</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'New Clients'!$E$15:$I$15</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
@@ -204,7 +204,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -219,6 +219,15 @@
         <color indexed="64"/>
       </top>
       <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -244,7 +253,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="6" applyNumberFormat="1"/>
@@ -261,14 +270,16 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="14" applyFont="1"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="17" applyFont="1"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="7" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="15" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="8" fontId="1" fillId="0" borderId="0" xfId="7" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="10" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="1" xfId="7" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="15" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="2" xfId="17" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="2" xfId="7" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="18">
     <cellStyle name="3wOifN/WbTHUMFiLTgs/6g9Ozr3TEGvhB0gQf6kN/CE=-~vV1U8Ka/jzyRgYU7x41wCw==" xfId="15"/>
@@ -558,7 +569,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -568,8 +579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView showFormulas="1" tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,18 +598,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="27" x14ac:dyDescent="0.35">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -666,34 +677,34 @@
       <c r="J5" s="3"/>
     </row>
     <row r="6" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="G6" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="H6" s="13" t="s">
         <v>34</v>
       </c>
       <c r="I6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="14" t="s">
+      <c r="J6" s="13" t="s">
         <v>35</v>
       </c>
     </row>
@@ -722,7 +733,7 @@
         <f>IF(D7="Yes",E7+F7,E7)</f>
         <v>725</v>
       </c>
-      <c r="H7" s="13">
+      <c r="H7" s="12">
         <f>$B$5*G7</f>
         <v>72.5</v>
       </c>
@@ -730,7 +741,7 @@
         <f>G7-H7</f>
         <v>652.5</v>
       </c>
-      <c r="J7" s="13">
+      <c r="J7" s="12">
         <f>-PMT($B$3/12,$B$4,I7)</f>
         <v>56.008501933458099</v>
       </c>
@@ -760,7 +771,7 @@
         <f t="shared" ref="G8:G14" si="2">IF(D8="Yes",E8+F8,E8)</f>
         <v>750</v>
       </c>
-      <c r="H8" s="13">
+      <c r="H8" s="12">
         <f t="shared" ref="H8:H14" si="3">$B$5*G8</f>
         <v>75</v>
       </c>
@@ -768,7 +779,7 @@
         <f t="shared" ref="I8:I14" si="4">G8-H8</f>
         <v>675</v>
       </c>
-      <c r="J8" s="13">
+      <c r="J8" s="12">
         <f t="shared" ref="J8:J14" si="5">-PMT($B$3/12,$B$4,I8)</f>
         <v>57.939829586335961</v>
       </c>
@@ -798,7 +809,7 @@
         <f t="shared" si="2"/>
         <v>475</v>
       </c>
-      <c r="H9" s="13">
+      <c r="H9" s="12">
         <f t="shared" si="3"/>
         <v>47.5</v>
       </c>
@@ -806,7 +817,7 @@
         <f t="shared" si="4"/>
         <v>427.5</v>
       </c>
-      <c r="J9" s="13">
+      <c r="J9" s="12">
         <f t="shared" si="5"/>
         <v>36.695225404679441</v>
       </c>
@@ -836,7 +847,7 @@
         <f t="shared" si="2"/>
         <v>300</v>
       </c>
-      <c r="H10" s="13">
+      <c r="H10" s="12">
         <f t="shared" si="3"/>
         <v>30</v>
       </c>
@@ -844,7 +855,7 @@
         <f t="shared" si="4"/>
         <v>270</v>
       </c>
-      <c r="J10" s="13">
+      <c r="J10" s="12">
         <f t="shared" si="5"/>
         <v>23.175931834534385</v>
       </c>
@@ -874,7 +885,7 @@
         <f t="shared" si="2"/>
         <v>725</v>
       </c>
-      <c r="H11" s="13">
+      <c r="H11" s="12">
         <f t="shared" si="3"/>
         <v>72.5</v>
       </c>
@@ -882,7 +893,7 @@
         <f t="shared" si="4"/>
         <v>652.5</v>
       </c>
-      <c r="J11" s="13">
+      <c r="J11" s="12">
         <f t="shared" si="5"/>
         <v>56.008501933458099</v>
       </c>
@@ -912,7 +923,7 @@
         <f t="shared" si="2"/>
         <v>475</v>
       </c>
-      <c r="H12" s="13">
+      <c r="H12" s="12">
         <f t="shared" si="3"/>
         <v>47.5</v>
       </c>
@@ -920,7 +931,7 @@
         <f t="shared" si="4"/>
         <v>427.5</v>
       </c>
-      <c r="J12" s="13">
+      <c r="J12" s="12">
         <f t="shared" si="5"/>
         <v>36.695225404679441</v>
       </c>
@@ -950,7 +961,7 @@
         <f t="shared" si="2"/>
         <v>175</v>
       </c>
-      <c r="H13" s="13">
+      <c r="H13" s="12">
         <f t="shared" si="3"/>
         <v>17.5</v>
       </c>
@@ -958,7 +969,7 @@
         <f t="shared" si="4"/>
         <v>157.5</v>
       </c>
-      <c r="J13" s="13">
+      <c r="J13" s="12">
         <f t="shared" si="5"/>
         <v>13.519293570145058</v>
       </c>
@@ -976,19 +987,19 @@
       <c r="D14" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="16">
         <f t="shared" si="0"/>
         <v>300</v>
       </c>
-      <c r="F14" s="10">
+      <c r="F14" s="16">
         <f t="shared" si="1"/>
         <v>275</v>
       </c>
-      <c r="G14" s="11">
+      <c r="G14" s="17">
         <f t="shared" si="2"/>
         <v>575</v>
       </c>
-      <c r="H14" s="13">
+      <c r="H14" s="12">
         <f t="shared" si="3"/>
         <v>57.5</v>
       </c>
@@ -996,7 +1007,7 @@
         <f t="shared" si="4"/>
         <v>517.5</v>
       </c>
-      <c r="J14" s="13">
+      <c r="J14" s="12">
         <f t="shared" si="5"/>
         <v>44.420536016190908</v>
       </c>
@@ -1007,27 +1018,27 @@
       <c r="D15" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="15">
+      <c r="E15" s="14">
         <f>SUM(E7:E14)</f>
         <v>2275</v>
       </c>
-      <c r="F15" s="15">
+      <c r="F15" s="14">
         <f t="shared" ref="F15:J15" si="6">SUM(F7:F14)</f>
         <v>2450</v>
       </c>
-      <c r="G15" s="15">
+      <c r="G15" s="14">
         <f t="shared" si="6"/>
         <v>4200</v>
       </c>
-      <c r="H15" s="15">
+      <c r="H15" s="14">
         <f t="shared" si="6"/>
         <v>420</v>
       </c>
-      <c r="I15" s="15">
+      <c r="I15" s="14">
         <f t="shared" si="6"/>
         <v>3780</v>
       </c>
-      <c r="J15" s="15">
+      <c r="J15" s="14">
         <f t="shared" si="6"/>
         <v>324.46304568348143</v>
       </c>
@@ -1069,13 +1080,13 @@
       <c r="J18" s="3"/>
     </row>
     <row r="19" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="13" t="s">
         <v>32</v>
       </c>
       <c r="D19" s="3"/>
@@ -1209,6 +1220,9 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;LDiksha Bansal&amp;C&amp;D&amp;R&amp;T</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 

</xml_diff>